<commit_message>
Utils, AWS, Groovy, Maven
Utils, AWS, Groovy, Maven
</commit_message>
<xml_diff>
--- a/Definitions/a_Definitions_Util.xlsx
+++ b/Definitions/a_Definitions_Util.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Topics" sheetId="3" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>Util Methods</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>Topics</t>
+  </si>
+  <si>
+    <t>Definitions</t>
   </si>
 </sst>
 </file>
@@ -153,7 +156,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -172,8 +175,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0066FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -231,6 +240,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="9" tint="-0.499984740745262"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="9" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -239,7 +274,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -263,8 +298,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -561,10 +605,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:A3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -572,12 +617,20 @@
     <col min="1" max="1" width="37.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1">
+    <row r="1" spans="1:2">
+      <c r="A1" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:2">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
@@ -586,6 +639,7 @@
   <hyperlinks>
     <hyperlink ref="A3" location="Date!A1" display="Date"/>
     <hyperlink ref="A2" location="RandomNumbers!A1" display="Random Numbers"/>
+    <hyperlink ref="B1" location="Topics!A2" display="Up"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -595,19 +649,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="55.125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="128.875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="105.875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -615,10 +669,10 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5"/>
+      <c r="B2" s="12"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
@@ -691,7 +745,7 @@
     <mergeCell ref="A12:A14"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B1" location="Utils!A2" display="Up"/>
+    <hyperlink ref="B1" location="RandomNumbers!A2" display="Up"/>
     <hyperlink ref="B3" r:id="rId1"/>
     <hyperlink ref="A1" location="Topics!A2" display="Topics"/>
   </hyperlinks>
@@ -703,9 +757,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -715,12 +769,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="12"/>
     </row>
     <row r="3" spans="1:2" ht="60">
       <c r="A3" s="8" t="s">
@@ -737,8 +797,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A2:B2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B1" location="Date!A2" display="Up"/>

</xml_diff>